<commit_message>
Update April 1, 2020
</commit_message>
<xml_diff>
--- a/Nasional/Old_backup/06_Nasional_Dead_29032020.xlsx
+++ b/Nasional/Old_backup/06_Nasional_Dead_29032020.xlsx
@@ -136,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -149,9 +149,6 @@
     </font>
     <font>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -194,10 +191,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1240,10 +1237,7 @@
       </c>
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
-      <c r="AD17" s="5">
-        <f>sum(AC12:AC16)</f>
-        <v>20</v>
-      </c>
+      <c r="AD17" s="5"/>
       <c r="AE17" s="5"/>
       <c r="AF17" s="5"/>
       <c r="AG17" s="5"/>

</xml_diff>